<commit_message>
css image page membres
</commit_message>
<xml_diff>
--- a/wp-content/themes/EchoPixels/information membres.xlsx
+++ b/wp-content/themes/EchoPixels/information membres.xlsx
@@ -236,7 +236,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -247,6 +247,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -531,7 +532,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,7 +630,9 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="G5" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="H5" s="1" t="s">
         <v>36</v>
       </c>
@@ -645,9 +648,7 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="5" t="s">
-        <v>44</v>
-      </c>
+      <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -774,7 +775,7 @@
         <v>29</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="2"/>
@@ -794,8 +795,9 @@
     <hyperlink ref="D15" r:id="rId4"/>
     <hyperlink ref="G15" r:id="rId5"/>
     <hyperlink ref="F15" r:id="rId6" display="https://twitter.com/Bertrand_Web"/>
+    <hyperlink ref="G5" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajout profile nicola et melinda
</commit_message>
<xml_diff>
--- a/wp-content/themes/EchoPixels/information membres.xlsx
+++ b/wp-content/themes/EchoPixels/information membres.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t xml:space="preserve">Tatiana            </t>
   </si>
@@ -159,13 +159,28 @@
   </si>
   <si>
     <t>https://www.linkedin.com/in/carinehalbout/</t>
+  </si>
+  <si>
+    <t>http://nikola7654.wixsite.com/monsite</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/nicolas-blavet-666285136/</t>
+  </si>
+  <si>
+    <t>www.mekabull.fr</t>
+  </si>
+  <si>
+    <t>https://fr.linkedin.com/in/melinda-khammar-868885133</t>
+  </si>
+  <si>
+    <t>https://twitter.com/mekabulle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,6 +192,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -236,7 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -248,6 +270,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -532,7 +557,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,11 +635,17 @@
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="11" t="s">
+        <v>47</v>
+      </c>
       <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="F4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="H4" s="5" t="s">
         <v>36</v>
       </c>
@@ -645,10 +676,14 @@
         <v>5</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="D6" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="9"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="G6" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -796,8 +831,11 @@
     <hyperlink ref="G15" r:id="rId5"/>
     <hyperlink ref="F15" r:id="rId6" display="https://twitter.com/Bertrand_Web"/>
     <hyperlink ref="G5" r:id="rId7"/>
+    <hyperlink ref="D6" r:id="rId8"/>
+    <hyperlink ref="G6" r:id="rId9"/>
+    <hyperlink ref="D4" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modificatino page membre prenom nom
</commit_message>
<xml_diff>
--- a/wp-content/themes/EchoPixels/information membres.xlsx
+++ b/wp-content/themes/EchoPixels/information membres.xlsx
@@ -557,7 +557,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,7 +711,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="2"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="11" t="s">
         <v>43</v>
       </c>
       <c r="H8" s="5"/>
@@ -824,18 +824,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G12" r:id="rId1" display="http://www.linkedin.com/in/alexandre-blin-bb637ab7"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="F3" r:id="rId3"/>
-    <hyperlink ref="D15" r:id="rId4"/>
-    <hyperlink ref="G15" r:id="rId5"/>
-    <hyperlink ref="F15" r:id="rId6" display="https://twitter.com/Bertrand_Web"/>
-    <hyperlink ref="G5" r:id="rId7"/>
-    <hyperlink ref="D6" r:id="rId8"/>
-    <hyperlink ref="G6" r:id="rId9"/>
-    <hyperlink ref="D4" r:id="rId10"/>
+    <hyperlink ref="G3" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F15" r:id="rId3" display="https://twitter.com/Bertrand_Web"/>
+    <hyperlink ref="G8" r:id="rId4"/>
+    <hyperlink ref="G12" r:id="rId5" display="http://www.linkedin.com/in/alexandre-blin-bb637ab7"/>
+    <hyperlink ref="G6" r:id="rId6"/>
+    <hyperlink ref="D6" r:id="rId7"/>
+    <hyperlink ref="D4" r:id="rId8"/>
+    <hyperlink ref="G15" r:id="rId9"/>
+    <hyperlink ref="D15" r:id="rId10"/>
+    <hyperlink ref="G5" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modification adresse site melinda tableau
</commit_message>
<xml_diff>
--- a/wp-content/themes/EchoPixels/information membres.xlsx
+++ b/wp-content/themes/EchoPixels/information membres.xlsx
@@ -167,13 +167,13 @@
     <t>https://www.linkedin.com/in/nicolas-blavet-666285136/</t>
   </si>
   <si>
-    <t>www.mekabull.fr</t>
-  </si>
-  <si>
     <t>https://fr.linkedin.com/in/melinda-khammar-868885133</t>
   </si>
   <si>
     <t>https://twitter.com/mekabulle</t>
+  </si>
+  <si>
+    <t>www.mekabulle.fr</t>
   </si>
 </sst>
 </file>
@@ -557,7 +557,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,14 +637,14 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
ajout information malory dans tableau
</commit_message>
<xml_diff>
--- a/wp-content/themes/EchoPixels/information membres.xlsx
+++ b/wp-content/themes/EchoPixels/information membres.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
   <si>
     <t xml:space="preserve">Tatiana            </t>
   </si>
@@ -174,6 +174,15 @@
   </si>
   <si>
     <t>https://twitter.com/mekabulle</t>
+  </si>
+  <si>
+    <t>Durand</t>
+  </si>
+  <si>
+    <t>Mallory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/mallory-durand-a71884133/ </t>
   </si>
 </sst>
 </file>
@@ -554,7 +563,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
@@ -822,6 +831,22 @@
       </c>
       <c r="H15" s="1"/>
     </row>
+    <row r="16" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" s="5"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G12" r:id="rId1" display="http://www.linkedin.com/in/alexandre-blin-bb637ab7"/>
@@ -834,8 +859,9 @@
     <hyperlink ref="D6" r:id="rId8"/>
     <hyperlink ref="G6" r:id="rId9"/>
     <hyperlink ref="D4" r:id="rId10"/>
+    <hyperlink ref="G16" r:id="rId11" display="https://www.linkedin.com/in/mallory-durand-a71884133/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>